<commit_message>
Added materials from meeting.
</commit_message>
<xml_diff>
--- a/Data/clean/Scorecards Clean - EXAMPLE.xlsx
+++ b/Data/clean/Scorecards Clean - EXAMPLE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendramarcoux/Library/CloudStorage/Box-Box/Legislative Scorecards/Data/clean/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cefayefang/Library/CloudStorage/Box-Box/Legislative Scorecards/Data/clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68B2F21-3F80-5043-BCF4-89EF196B8550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEF6015-60D9-904A-875F-0699E16CA322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="2" xr2:uid="{EFE6F266-E20E-3A47-983A-491ECE3CE1FF}"/>
+    <workbookView xWindow="1080" yWindow="760" windowWidth="29160" windowHeight="18880" xr2:uid="{EFE6F266-E20E-3A47-983A-491ECE3CE1FF}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="93">
   <si>
     <t>Year</t>
   </si>
@@ -286,6 +286,9 @@
     <t>Start with the Legislation tab for each new scorecard - as long as the PDF details which bills the house and the senate voted on in that cycle.</t>
   </si>
   <si>
+    <t xml:space="preserve">Record the state, year, title, and house (senate or not) for each bill. Use the year that the bill was actually voted on, dates should usually be included. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Add tags for each bill. Options are Agriculture, Energy, Climate, Conservation, Wildlife, Waste, and Other. </t>
   </si>
   <si>
@@ -314,15 +317,6 @@
   </si>
   <si>
     <t xml:space="preserve">If you have any questions, send me a slack message or an email :) </t>
-  </si>
-  <si>
-    <t>Party</t>
-  </si>
-  <si>
-    <t>Pictures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Record the state, year, title, and house (senate=1 or house=0) for each bill. Use the year that the bill was actually voted on, dates should usually be included. </t>
   </si>
 </sst>
 </file>
@@ -694,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ADA510-7EA1-FD4C-AD1C-282AC32FFCF3}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -707,57 +701,57 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -770,7 +764,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1127,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0734319C-46E1-6B43-95CA-FBADA7542208}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A16:XFD28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1138,18 +1132,16 @@
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1169,34 +1161,28 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>92</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1215,29 +1201,29 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="I2">
+      <c r="G2">
         <v>93</v>
       </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2" t="s">
+        <v>76</v>
+      </c>
       <c r="J2">
         <v>100</v>
       </c>
       <c r="K2" t="s">
         <v>76</v>
       </c>
-      <c r="L2">
-        <v>100</v>
-      </c>
-      <c r="M2" t="s">
-        <v>76</v>
-      </c>
-      <c r="N2" t="s">
-        <v>76</v>
-      </c>
-      <c r="O2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1256,29 +1242,29 @@
       <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="I3">
+      <c r="G3">
         <v>92</v>
       </c>
+      <c r="H3">
+        <v>100</v>
+      </c>
+      <c r="I3" t="s">
+        <v>76</v>
+      </c>
       <c r="J3">
         <v>100</v>
       </c>
       <c r="K3" t="s">
         <v>76</v>
       </c>
-      <c r="L3">
-        <v>100</v>
-      </c>
-      <c r="M3" t="s">
-        <v>76</v>
-      </c>
-      <c r="N3" t="s">
-        <v>76</v>
-      </c>
-      <c r="O3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1297,29 +1283,29 @@
       <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="I4">
+      <c r="G4">
         <v>86</v>
       </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+      <c r="I4" t="s">
+        <v>76</v>
+      </c>
       <c r="J4">
         <v>100</v>
       </c>
       <c r="K4" t="s">
         <v>76</v>
       </c>
-      <c r="L4">
-        <v>100</v>
-      </c>
-      <c r="M4" t="s">
-        <v>76</v>
-      </c>
-      <c r="N4" t="s">
-        <v>76</v>
-      </c>
-      <c r="O4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1338,29 +1324,29 @@
       <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="I5">
+      <c r="G5">
         <v>79</v>
       </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5" t="s">
+        <v>76</v>
+      </c>
       <c r="J5">
         <v>100</v>
       </c>
       <c r="K5" t="s">
         <v>76</v>
       </c>
-      <c r="L5">
-        <v>100</v>
-      </c>
-      <c r="M5" t="s">
-        <v>76</v>
-      </c>
-      <c r="N5" t="s">
-        <v>76</v>
-      </c>
-      <c r="O5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1379,29 +1365,29 @@
       <c r="F6" t="s">
         <v>26</v>
       </c>
-      <c r="I6">
+      <c r="G6">
         <v>79</v>
       </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6" t="s">
+        <v>76</v>
+      </c>
       <c r="J6">
         <v>100</v>
       </c>
       <c r="K6" t="s">
         <v>76</v>
       </c>
-      <c r="L6">
-        <v>100</v>
-      </c>
-      <c r="M6" t="s">
-        <v>76</v>
-      </c>
-      <c r="N6" t="s">
-        <v>76</v>
-      </c>
-      <c r="O6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L6" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1420,29 +1406,29 @@
       <c r="F7" t="s">
         <v>27</v>
       </c>
-      <c r="I7">
+      <c r="G7">
         <v>79</v>
       </c>
+      <c r="H7">
+        <v>100</v>
+      </c>
+      <c r="I7" t="s">
+        <v>76</v>
+      </c>
       <c r="J7">
         <v>100</v>
       </c>
       <c r="K7" t="s">
         <v>76</v>
       </c>
-      <c r="L7">
-        <v>100</v>
-      </c>
-      <c r="M7" t="s">
-        <v>76</v>
-      </c>
-      <c r="N7" t="s">
-        <v>76</v>
-      </c>
-      <c r="O7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L7" t="s">
+        <v>76</v>
+      </c>
+      <c r="M7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1461,29 +1447,29 @@
       <c r="F8" t="s">
         <v>28</v>
       </c>
-      <c r="I8">
+      <c r="G8">
         <v>79</v>
       </c>
+      <c r="H8">
+        <v>100</v>
+      </c>
+      <c r="I8" t="s">
+        <v>76</v>
+      </c>
       <c r="J8">
         <v>100</v>
       </c>
       <c r="K8" t="s">
         <v>76</v>
       </c>
-      <c r="L8">
-        <v>100</v>
-      </c>
-      <c r="M8" t="s">
-        <v>76</v>
-      </c>
-      <c r="N8" t="s">
-        <v>76</v>
-      </c>
-      <c r="O8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L8" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1502,29 +1488,29 @@
       <c r="F9" t="s">
         <v>71</v>
       </c>
-      <c r="I9">
+      <c r="G9">
         <v>77</v>
       </c>
+      <c r="H9">
+        <v>100</v>
+      </c>
+      <c r="I9" t="s">
+        <v>76</v>
+      </c>
       <c r="J9">
         <v>100</v>
       </c>
       <c r="K9" t="s">
         <v>76</v>
       </c>
-      <c r="L9">
-        <v>100</v>
-      </c>
-      <c r="M9" t="s">
-        <v>76</v>
-      </c>
-      <c r="N9" t="s">
-        <v>76</v>
-      </c>
-      <c r="O9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L9" t="s">
+        <v>76</v>
+      </c>
+      <c r="M9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1543,29 +1529,29 @@
       <c r="F10" t="s">
         <v>72</v>
       </c>
-      <c r="I10">
+      <c r="G10">
         <v>71</v>
       </c>
+      <c r="H10">
+        <v>100</v>
+      </c>
+      <c r="I10" t="s">
+        <v>76</v>
+      </c>
       <c r="J10">
         <v>100</v>
       </c>
       <c r="K10" t="s">
         <v>76</v>
       </c>
-      <c r="L10">
-        <v>100</v>
-      </c>
-      <c r="M10" t="s">
-        <v>76</v>
-      </c>
-      <c r="N10" t="s">
-        <v>76</v>
-      </c>
-      <c r="O10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L10" t="s">
+        <v>76</v>
+      </c>
+      <c r="M10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1584,29 +1570,29 @@
       <c r="F11" t="s">
         <v>73</v>
       </c>
-      <c r="I11">
+      <c r="G11">
         <v>71</v>
       </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
+      <c r="I11" t="s">
+        <v>76</v>
+      </c>
       <c r="J11">
         <v>100</v>
       </c>
       <c r="K11" t="s">
         <v>76</v>
       </c>
-      <c r="L11">
-        <v>100</v>
-      </c>
-      <c r="M11" t="s">
-        <v>76</v>
-      </c>
-      <c r="N11" t="s">
-        <v>76</v>
-      </c>
-      <c r="O11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1625,29 +1611,29 @@
       <c r="F12" t="s">
         <v>74</v>
       </c>
-      <c r="I12">
+      <c r="G12">
         <v>71</v>
       </c>
+      <c r="H12">
+        <v>100</v>
+      </c>
+      <c r="I12" t="s">
+        <v>76</v>
+      </c>
       <c r="J12">
         <v>100</v>
       </c>
       <c r="K12" t="s">
         <v>76</v>
       </c>
-      <c r="L12">
-        <v>100</v>
-      </c>
-      <c r="M12" t="s">
-        <v>76</v>
-      </c>
-      <c r="N12" t="s">
-        <v>76</v>
-      </c>
-      <c r="O12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L12" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1666,29 +1652,29 @@
       <c r="F13" t="s">
         <v>75</v>
       </c>
-      <c r="I13">
+      <c r="G13">
         <v>71</v>
       </c>
+      <c r="H13">
+        <v>100</v>
+      </c>
+      <c r="I13" t="s">
+        <v>76</v>
+      </c>
       <c r="J13">
         <v>100</v>
       </c>
       <c r="K13" t="s">
         <v>76</v>
       </c>
-      <c r="L13">
-        <v>100</v>
-      </c>
-      <c r="M13" t="s">
-        <v>76</v>
-      </c>
-      <c r="N13" t="s">
-        <v>76</v>
-      </c>
-      <c r="O13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1707,34 +1693,34 @@
       <c r="F14" t="s">
         <v>80</v>
       </c>
-      <c r="I14">
+      <c r="G14">
         <v>64</v>
       </c>
+      <c r="H14">
+        <v>100</v>
+      </c>
+      <c r="I14" t="s">
+        <v>76</v>
+      </c>
       <c r="J14">
         <v>100</v>
       </c>
       <c r="K14" t="s">
         <v>76</v>
       </c>
-      <c r="L14">
-        <v>100</v>
-      </c>
-      <c r="M14" t="s">
-        <v>76</v>
-      </c>
-      <c r="N14" t="s">
-        <v>76</v>
-      </c>
-      <c r="O14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L14" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1753,8 +1739,14 @@
       <c r="F16" t="s">
         <v>10</v>
       </c>
+      <c r="G16">
+        <v>93</v>
+      </c>
+      <c r="H16">
+        <v>100</v>
+      </c>
       <c r="I16">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="J16">
         <v>100</v>
@@ -1765,17 +1757,11 @@
       <c r="L16">
         <v>100</v>
       </c>
-      <c r="M16">
-        <v>100</v>
-      </c>
-      <c r="N16">
-        <v>100</v>
-      </c>
-      <c r="O16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1794,8 +1780,14 @@
       <c r="F17" t="s">
         <v>13</v>
       </c>
+      <c r="G17">
+        <v>92</v>
+      </c>
+      <c r="H17">
+        <v>100</v>
+      </c>
       <c r="I17">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J17">
         <v>100</v>
@@ -1806,17 +1798,11 @@
       <c r="L17">
         <v>100</v>
       </c>
-      <c r="M17">
-        <v>100</v>
-      </c>
-      <c r="N17">
-        <v>100</v>
-      </c>
-      <c r="O17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1835,8 +1821,14 @@
       <c r="F18" t="s">
         <v>16</v>
       </c>
+      <c r="G18">
+        <v>86</v>
+      </c>
+      <c r="H18">
+        <v>100</v>
+      </c>
       <c r="I18">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="J18">
         <v>100</v>
@@ -1847,17 +1839,11 @@
       <c r="L18">
         <v>100</v>
       </c>
-      <c r="M18">
-        <v>100</v>
-      </c>
-      <c r="N18">
-        <v>100</v>
-      </c>
-      <c r="O18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1876,8 +1862,14 @@
       <c r="F19" t="s">
         <v>19</v>
       </c>
+      <c r="G19">
+        <v>79</v>
+      </c>
+      <c r="H19">
+        <v>100</v>
+      </c>
       <c r="I19">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="J19">
         <v>100</v>
@@ -1888,17 +1880,11 @@
       <c r="L19">
         <v>100</v>
       </c>
-      <c r="M19">
-        <v>100</v>
-      </c>
-      <c r="N19">
-        <v>100</v>
-      </c>
-      <c r="O19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1917,8 +1903,14 @@
       <c r="F20" t="s">
         <v>26</v>
       </c>
+      <c r="G20">
+        <v>79</v>
+      </c>
+      <c r="H20">
+        <v>100</v>
+      </c>
       <c r="I20">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="J20">
         <v>100</v>
@@ -1929,17 +1921,11 @@
       <c r="L20">
         <v>100</v>
       </c>
-      <c r="M20">
-        <v>100</v>
-      </c>
-      <c r="N20">
-        <v>100</v>
-      </c>
-      <c r="O20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1958,8 +1944,14 @@
       <c r="F21" t="s">
         <v>27</v>
       </c>
+      <c r="G21">
+        <v>79</v>
+      </c>
+      <c r="H21">
+        <v>100</v>
+      </c>
       <c r="I21">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="J21">
         <v>100</v>
@@ -1970,17 +1962,11 @@
       <c r="L21">
         <v>100</v>
       </c>
-      <c r="M21">
-        <v>100</v>
-      </c>
-      <c r="N21">
-        <v>100</v>
-      </c>
-      <c r="O21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1999,8 +1985,14 @@
       <c r="F22" t="s">
         <v>28</v>
       </c>
+      <c r="G22">
+        <v>79</v>
+      </c>
+      <c r="H22">
+        <v>100</v>
+      </c>
       <c r="I22">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="J22">
         <v>100</v>
@@ -2011,17 +2003,11 @@
       <c r="L22">
         <v>100</v>
       </c>
-      <c r="M22">
-        <v>100</v>
-      </c>
-      <c r="N22">
-        <v>100</v>
-      </c>
-      <c r="O22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -2040,8 +2026,14 @@
       <c r="F23" t="s">
         <v>71</v>
       </c>
+      <c r="G23">
+        <v>77</v>
+      </c>
+      <c r="H23">
+        <v>100</v>
+      </c>
       <c r="I23">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="J23">
         <v>100</v>
@@ -2052,17 +2044,11 @@
       <c r="L23">
         <v>100</v>
       </c>
-      <c r="M23">
-        <v>100</v>
-      </c>
-      <c r="N23">
-        <v>100</v>
-      </c>
-      <c r="O23" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2081,8 +2067,14 @@
       <c r="F24" t="s">
         <v>72</v>
       </c>
+      <c r="G24">
+        <v>71</v>
+      </c>
+      <c r="H24">
+        <v>100</v>
+      </c>
       <c r="I24">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="J24">
         <v>100</v>
@@ -2093,17 +2085,11 @@
       <c r="L24">
         <v>100</v>
       </c>
-      <c r="M24">
-        <v>100</v>
-      </c>
-      <c r="N24">
-        <v>100</v>
-      </c>
-      <c r="O24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -2122,8 +2108,14 @@
       <c r="F25" t="s">
         <v>73</v>
       </c>
+      <c r="G25">
+        <v>71</v>
+      </c>
+      <c r="H25">
+        <v>100</v>
+      </c>
       <c r="I25">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="J25">
         <v>100</v>
@@ -2134,17 +2126,11 @@
       <c r="L25">
         <v>100</v>
       </c>
-      <c r="M25">
-        <v>100</v>
-      </c>
-      <c r="N25">
-        <v>100</v>
-      </c>
-      <c r="O25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -2163,8 +2149,14 @@
       <c r="F26" t="s">
         <v>74</v>
       </c>
+      <c r="G26">
+        <v>71</v>
+      </c>
+      <c r="H26">
+        <v>100</v>
+      </c>
       <c r="I26">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="J26">
         <v>100</v>
@@ -2175,17 +2167,11 @@
       <c r="L26">
         <v>100</v>
       </c>
-      <c r="M26">
-        <v>100</v>
-      </c>
-      <c r="N26">
-        <v>100</v>
-      </c>
-      <c r="O26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -2204,8 +2190,14 @@
       <c r="F27" t="s">
         <v>75</v>
       </c>
+      <c r="G27">
+        <v>71</v>
+      </c>
+      <c r="H27">
+        <v>100</v>
+      </c>
       <c r="I27">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="J27">
         <v>100</v>
@@ -2216,17 +2208,11 @@
       <c r="L27">
         <v>100</v>
       </c>
-      <c r="M27">
-        <v>100</v>
-      </c>
-      <c r="N27">
-        <v>100</v>
-      </c>
-      <c r="O27" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -2245,25 +2231,25 @@
       <c r="F28" t="s">
         <v>80</v>
       </c>
+      <c r="G28">
+        <v>64</v>
+      </c>
+      <c r="H28">
+        <v>100</v>
+      </c>
       <c r="I28">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="J28">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K28">
         <v>100</v>
       </c>
       <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <v>100</v>
-      </c>
-      <c r="N28">
-        <v>100</v>
-      </c>
-      <c r="O28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M28" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>